<commit_message>
Figure changes and measurement calculations
</commit_message>
<xml_diff>
--- a/Measurements/TrialMeasurements.xlsx
+++ b/Measurements/TrialMeasurements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -32,21 +32,6 @@
     <t>Data TIWSNE - Measurements</t>
   </si>
   <si>
-    <t>Voltage [mV]</t>
-  </si>
-  <si>
-    <t>Shunt Resistor [Ohm]</t>
-  </si>
-  <si>
-    <t>Current [mA]</t>
-  </si>
-  <si>
-    <t>Power [W]</t>
-  </si>
-  <si>
-    <t>Battery Voltage [V]</t>
-  </si>
-  <si>
     <t>Time [s]</t>
   </si>
   <si>
@@ -81,6 +66,21 @@
   </si>
   <si>
     <t>Fra idle til receiver circuit</t>
+  </si>
+  <si>
+    <t>Ushunt [mV]</t>
+  </si>
+  <si>
+    <t>Rshunt [Ohm]</t>
+  </si>
+  <si>
+    <t>Imote[mA]</t>
+  </si>
+  <si>
+    <t>Ubattery [V]</t>
+  </si>
+  <si>
+    <t>Pmote [W]</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,30 +417,30 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -456,19 +456,19 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <f>(E4-(B4*0.001))*(B4*0.001)</f>
-        <v>5.96E-2</v>
+        <f>(E4-(B4*0.001))*(B4*0.001)/10</f>
+        <v>5.96E-3</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>181.25</v>
@@ -484,19 +484,19 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <f>(E5-(B5*0.001))*(B5*0.001)</f>
-        <v>0.51089843749999997</v>
+        <f t="shared" ref="F5:F11" si="0">(E5-(B5*0.001))*(B5*0.001)/10</f>
+        <v>5.1089843749999996E-2</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>176.25</v>
@@ -505,26 +505,26 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:D14" si="0">B6/C6</f>
+        <f t="shared" ref="D6:D14" si="1">B6/C6</f>
         <v>17.625</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <f>(E6-(B6*0.001))*(B6*0.001)</f>
-        <v>0.49768593749999995</v>
+        <f t="shared" si="0"/>
+        <v>4.9768593749999993E-2</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -533,43 +533,43 @@
         <v>10</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <f>(E7-(B7*0.001))*(B7*0.001)</f>
-        <v>5.96E-2</v>
+        <v>5.96E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>189</v>
+        <v>188.75</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>18.875</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <f>(E8-(B8*0.001))*(B8*0.001)</f>
-        <v>0.53127899999999995</v>
+        <v>5.3062343749999998E-2</v>
       </c>
       <c r="H8">
         <f>F8*G8</f>
@@ -578,7 +578,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>220</v>
@@ -587,15 +587,15 @@
         <v>10</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <f>(E9-(B9*0.001))*(B9*0.001)</f>
-        <v>0.61159999999999992</v>
+        <v>6.1159999999999992E-2</v>
       </c>
       <c r="H9">
         <f>F9*G9</f>
@@ -604,36 +604,36 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>189</v>
+        <v>188.75</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>18.899999999999999</v>
+        <f t="shared" si="1"/>
+        <v>18.875</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F6:F14" si="1">(E10-(B10*0.001))*(B10*0.001)</f>
-        <v>0.53127899999999995</v>
+        <f>(E10-(B10*0.001))*(B10*0.001)/10</f>
+        <v>5.3062343749999998E-2</v>
       </c>
       <c r="G10">
         <v>43</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H7:H14" si="2">F10*G10</f>
-        <v>22.844996999999999</v>
+        <f>F10*G10</f>
+        <v>2.28168078125</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>191</v>
@@ -642,22 +642,22 @@
         <v>10</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>19.100000000000001</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>0.53651900000000008</v>
+        <v>5.3651900000000009E-2</v>
       </c>
       <c r="G11">
         <v>24.5</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>13.144715500000002</v>
+        <f t="shared" ref="H11:H14" si="2">F11*G11</f>
+        <v>1.3144715500000002</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -665,14 +665,14 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E12">
         <v>3</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F12:F14" si="3">(E12-(B12*0.001))*(B12*0.001)</f>
         <v>0</v>
       </c>
       <c r="H12">
@@ -685,14 +685,14 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13">
@@ -705,14 +705,14 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14">
@@ -722,7 +722,7 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>